<commit_message>
Changes for 1.0.3 release.
- Improved authentication algorithm
- Clarify authentication exception messages
- Added config comments regarding authentication types
- Renamed command-line options:
    - -e 'Filter' -f
    - -d 'Search String' to -s
    - -g 'Debug' to -d
    - -s 'Sudo' to -u
- Check for file existence of SSH_PRIVATE_KEY_FILE if defined as #
- Test support for RSA key with and without a passphrase
- Added new config option SSH_AGENT_ONLY to force ssh-agent only authentication
- Separate authentication/connection exception messages
</commit_message>
<xml_diff>
--- a/docs/templates/commands_template.xlsx
+++ b/docs/templates/commands_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randyo/dev/Nova/docs/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m173404/dev/repos/github/reach/docs/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA926B05-C6D7-2E4A-AC64-73BCFA73DA92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3440" windowWidth="26180" windowHeight="17180" tabRatio="500"/>
+    <workbookView xWindow="6620" yWindow="2740" windowWidth="26180" windowHeight="17180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batch_cmds_template.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,28 +66,28 @@
     <t>Show Output (-o) (Default = no)</t>
   </si>
   <si>
-    <t>Send (-p) String(s)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expect (-w) String(s) </t>
   </si>
   <si>
     <t>Print Status (-r)</t>
   </si>
   <si>
-    <t>Search (-d) String(s)</t>
-  </si>
-  <si>
     <t>Halt (-h) hosts loop when found Search String (Default = no)</t>
   </si>
   <si>
     <t>Command (Can use host file column $HF_#. For example: $HF_8 (use data from 8th column of hosts file)</t>
+  </si>
+  <si>
+    <t>Put (-p) String(s)</t>
+  </si>
+  <si>
+    <t>Search (-s) String(s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -138,6 +139,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,7 +409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -421,9 +425,9 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -432,19 +436,19 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>